<commit_message>
Updated xlsx loader and his tests, changed fingerscrossed extractor and updated csv tests
</commit_message>
<xml_diff>
--- a/tests/functional/Sheet/source-to-extract.xlsx
+++ b/tests/functional/Sheet/source-to-extract.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,64 +112,71 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.24489795918367"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>